<commit_message>
Fix Style Results Files Gemma
</commit_message>
<xml_diff>
--- a/Results/gemma/final_tasks_generated_anonymous.xlsx
+++ b/Results/gemma/final_tasks_generated_anonymous.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniocurci/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniocurci/Developer/GitHub/code-paper/results/gemma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC9E6C-D324-DC42-B802-BD1834D616EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69885EDE-DE16-484E-8FF7-C8E112C916CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="38160" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="760" windowWidth="16440" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -7644,7 +7644,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -7655,6 +7678,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E2CCB2F-F0E5-DC49-BC0D-C5249A2D378A}" name="Table1" displayName="Table1" ref="A1:D2881" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D2881" xr:uid="{4E2CCB2F-F0E5-DC49-BC0D-C5249A2D378A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{940B3D8B-A949-C74D-A163-FCD3740BC85C}" name="prompt_type"/>
+    <tableColumn id="2" xr3:uid="{C70B8A7B-7213-624A-8AF2-1F7B602E455B}" name="temperature"/>
+    <tableColumn id="3" xr3:uid="{3B229295-8CAA-A54D-AE5B-BD54F818EC07}" name="generation"/>
+    <tableColumn id="4" xr3:uid="{D767D79B-59E5-F84D-8E96-8359E7590B2D}" name="task" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7946,8 +7982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2881"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2349" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2232" sqref="D2232"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7993,7 +8029,9 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5">
+        <v>6</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
@@ -8005,7 +8043,9 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5">
+        <v>6</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
@@ -8017,7 +8057,9 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5">
+        <v>6</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
@@ -8029,7 +8071,9 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5">
+        <v>6</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
@@ -8041,7 +8085,9 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>6</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
@@ -8053,7 +8099,9 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5">
+        <v>6</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
@@ -48231,12 +48279,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="C953:C961"/>
-    <mergeCell ref="C1142:C1151"/>
-    <mergeCell ref="C2231:C2239"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>